<commit_message>
Generation Formulaes for fileds added
</commit_message>
<xml_diff>
--- a/Endpoints.xlsx
+++ b/Endpoints.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Environment\DEV\Documentation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Environment\DEV\Documentation\stock-project-documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE331A86-D7B1-4AAA-BA4D-B9B166B7C61F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0CF7C71-D233-42E4-82E4-10EB57D07DC9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{30700010-F763-4196-BFD8-63DDF9783492}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="256" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="294" uniqueCount="100">
   <si>
     <t>Class</t>
   </si>
@@ -284,10 +284,76 @@
     <t>Overall Sold Amount</t>
   </si>
   <si>
-    <t>Return Per Transaction</t>
-  </si>
-  <si>
     <t>Summary Dashboard</t>
+  </si>
+  <si>
+    <t>Generation Formula</t>
+  </si>
+  <si>
+    <t>sum(buyPrice*quantity) from stocks table</t>
+  </si>
+  <si>
+    <t>sum(regularMarketPrice*quantity) from current holding api response</t>
+  </si>
+  <si>
+    <t>overall current value - overall investment value</t>
+  </si>
+  <si>
+    <t>(overall current value - overall investment value)*100/overall current value</t>
+  </si>
+  <si>
+    <t>latest(investmentDate) from stocks table</t>
+  </si>
+  <si>
+    <t>Fetch from db</t>
+  </si>
+  <si>
+    <t>sum(sellPrice) - sum(buyPrice)  from profit-loss table</t>
+  </si>
+  <si>
+    <t>sum(buyPrice)  from profit-loss table</t>
+  </si>
+  <si>
+    <t>sum(sellPrice)  from profit-loss table</t>
+  </si>
+  <si>
+    <t>latest(investmentDate) from profit-loss table</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Average Return Per Transaction </t>
+  </si>
+  <si>
+    <t>Average Return Percent Per Transaction</t>
+  </si>
+  <si>
+    <t>(overall p/l - overall bought)/count(records) from profit-loss table</t>
+  </si>
+  <si>
+    <t>sum(creditedAmount) from dividend table</t>
+  </si>
+  <si>
+    <t>sum(creditedAmount) - sum(debitedAmount) from fund table</t>
+  </si>
+  <si>
+    <t>sum(creditedAmount) from fund table</t>
+  </si>
+  <si>
+    <t>sum(debitedAmount) from fund table</t>
+  </si>
+  <si>
+    <t>latest(creditedDate) from dividend table</t>
+  </si>
+  <si>
+    <t>latest(transactionDate) from fund table</t>
+  </si>
+  <si>
+    <t>sum(amountAdded) from mutual-fund table</t>
+  </si>
+  <si>
+    <t>regularMarketPrice from current holding api response</t>
+  </si>
+  <si>
+    <t>latest(investmentDate) from mutual-fund table</t>
   </si>
 </sst>
 </file>
@@ -323,7 +389,7 @@
       <family val="3"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -341,8 +407,13 @@
         <fgColor theme="4"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="7">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -418,13 +489,23 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="4"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -448,13 +529,81 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="3"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="3" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="3" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="7" xfId="3" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="4">
     <cellStyle name="Accent1" xfId="2" builtinId="29"/>
+    <cellStyle name="Accent3" xfId="3" builtinId="37"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="12">
+  <dxfs count="14">
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="thin">
+          <color theme="4"/>
+        </right>
+        <top style="thin">
+          <color theme="4"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="thin">
+          <color theme="4"/>
+        </right>
+        <top style="thin">
+          <color theme="4"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -729,78 +878,84 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{5458B2E5-FFC7-4C32-829A-E986A7A5E442}" name="Table2" displayName="Table2" ref="A26:D29" totalsRowShown="0">
-  <autoFilter ref="A26:D29" xr:uid="{5458B2E5-FFC7-4C32-829A-E986A7A5E442}"/>
-  <tableColumns count="4">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{5458B2E5-FFC7-4C32-829A-E986A7A5E442}" name="Table2" displayName="Table2" ref="A26:E29" totalsRowShown="0">
+  <autoFilter ref="A26:E29" xr:uid="{5458B2E5-FFC7-4C32-829A-E986A7A5E442}"/>
+  <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{688E3C3B-D317-4C98-A054-3BE5422EA63F}" name="Field"/>
     <tableColumn id="2" xr3:uid="{B511B556-A733-4517-8C85-34070BFC361B}" name="Updated Method"/>
     <tableColumn id="3" xr3:uid="{59E920CB-0533-4CE8-908B-0C7E19004603}" name="Storage Method"/>
     <tableColumn id="4" xr3:uid="{06FE7570-AA3C-48D2-8F0A-2E7E00298919}" name="Datatype"/>
+    <tableColumn id="5" xr3:uid="{B7C54223-7E16-496C-BCCF-87B18D195F88}" name="Generation Formula"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{0BFD4176-5F69-4875-BF59-293160C2EE86}" name="Table3" displayName="Table3" ref="A32:D37" totalsRowShown="0" tableBorderDxfId="11">
-  <autoFilter ref="A32:D37" xr:uid="{0BFD4176-5F69-4875-BF59-293160C2EE86}"/>
-  <tableColumns count="4">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{0BFD4176-5F69-4875-BF59-293160C2EE86}" name="Table3" displayName="Table3" ref="A32:E37" totalsRowShown="0" tableBorderDxfId="13">
+  <autoFilter ref="A32:E37" xr:uid="{0BFD4176-5F69-4875-BF59-293160C2EE86}"/>
+  <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{4FEFCDF2-FE87-456F-8582-283484542A4C}" name="Field"/>
     <tableColumn id="2" xr3:uid="{E37067D1-9308-49A6-951C-A0E4C1195265}" name="Updated Method"/>
     <tableColumn id="3" xr3:uid="{A870BFD7-27F4-40E5-A72B-A4CC431BE64F}" name="Storage Method"/>
     <tableColumn id="4" xr3:uid="{CC68BEF1-5A7D-4E13-80F5-40174E39F5A1}" name="Datatype"/>
+    <tableColumn id="5" xr3:uid="{0A1B7B91-9E94-4EE5-B841-DB66A0475DDB}" name="Generation Formula"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{3FD62E6F-799B-4C8C-8163-DCCDC99141A8}" name="Table4" displayName="Table4" ref="A40:D46" totalsRowShown="0" tableBorderDxfId="10">
-  <autoFilter ref="A40:D46" xr:uid="{3FD62E6F-799B-4C8C-8163-DCCDC99141A8}"/>
-  <tableColumns count="4">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{3FD62E6F-799B-4C8C-8163-DCCDC99141A8}" name="Table4" displayName="Table4" ref="A40:E46" totalsRowShown="0" tableBorderDxfId="12">
+  <autoFilter ref="A40:E46" xr:uid="{3FD62E6F-799B-4C8C-8163-DCCDC99141A8}"/>
+  <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{EBB6A018-4229-44E2-BFEC-5735124A49D6}" name="Field"/>
     <tableColumn id="2" xr3:uid="{FC54E304-E834-423E-9BAD-E6E45489B546}" name="Updated Method"/>
     <tableColumn id="3" xr3:uid="{613DDB66-D41E-4B6C-B527-E8DFC784E985}" name="Storage Method"/>
     <tableColumn id="4" xr3:uid="{9C6A3024-B511-49C3-B5CC-FCFDE9C75704}" name="Datatype"/>
+    <tableColumn id="5" xr3:uid="{A64F5098-7655-48F5-AF7E-F022BCE52994}" name="Generation Formula" dataCellStyle="Accent3"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{588681AB-2343-4772-8F61-01FB6DEA49BE}" name="Table6" displayName="Table6" ref="A49:D56" totalsRowShown="0" tableBorderDxfId="9">
-  <autoFilter ref="A49:D56" xr:uid="{588681AB-2343-4772-8F61-01FB6DEA49BE}"/>
-  <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{A46E78D4-40E3-4CC2-9E07-4DABCC13ECD1}" name="Field" dataDxfId="8"/>
-    <tableColumn id="2" xr3:uid="{8A2E0C0E-C378-49DE-BA9B-6CA0CCEAFBF3}" name="Updated Method" dataDxfId="7"/>
-    <tableColumn id="3" xr3:uid="{63A090DB-A088-4A75-AB57-104DB398EB6A}" name="Storage Method" dataDxfId="6"/>
-    <tableColumn id="4" xr3:uid="{DAC83841-7394-440C-B6AC-A9D73F43D271}" name="Datatype" dataDxfId="5"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{588681AB-2343-4772-8F61-01FB6DEA49BE}" name="Table6" displayName="Table6" ref="A49:E56" totalsRowShown="0" tableBorderDxfId="11">
+  <autoFilter ref="A49:E56" xr:uid="{588681AB-2343-4772-8F61-01FB6DEA49BE}"/>
+  <tableColumns count="5">
+    <tableColumn id="1" xr3:uid="{A46E78D4-40E3-4CC2-9E07-4DABCC13ECD1}" name="Field" dataDxfId="10"/>
+    <tableColumn id="2" xr3:uid="{8A2E0C0E-C378-49DE-BA9B-6CA0CCEAFBF3}" name="Updated Method" dataDxfId="9"/>
+    <tableColumn id="3" xr3:uid="{63A090DB-A088-4A75-AB57-104DB398EB6A}" name="Storage Method" dataDxfId="8"/>
+    <tableColumn id="4" xr3:uid="{DAC83841-7394-440C-B6AC-A9D73F43D271}" name="Datatype" dataDxfId="7"/>
+    <tableColumn id="5" xr3:uid="{DB5D1536-7619-490E-9FE4-86DA2FB10366}" name="Generation Formula" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{7E2565EE-2AC7-45FA-8DCC-4FA501A0CBAE}" name="Table7" displayName="Table7" ref="A59:D65" totalsRowShown="0">
-  <autoFilter ref="A59:D65" xr:uid="{7E2565EE-2AC7-45FA-8DCC-4FA501A0CBAE}"/>
-  <tableColumns count="4">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{7E2565EE-2AC7-45FA-8DCC-4FA501A0CBAE}" name="Table7" displayName="Table7" ref="A59:E66" totalsRowShown="0">
+  <autoFilter ref="A59:E66" xr:uid="{7E2565EE-2AC7-45FA-8DCC-4FA501A0CBAE}"/>
+  <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{C2B1F201-E24C-4440-A910-1D2DA6518B24}" name="Field"/>
     <tableColumn id="2" xr3:uid="{24B8A508-38BE-4BFD-A43A-7033CE93F7DF}" name="Updated Method"/>
     <tableColumn id="3" xr3:uid="{9A831C7C-F95F-4CE5-A352-41936EE80EEC}" name="Storage Method"/>
     <tableColumn id="4" xr3:uid="{2D5D09E6-B72E-47AC-92C5-4AE0287C67FB}" name="Datatype"/>
+    <tableColumn id="5" xr3:uid="{593FFB5A-2ED0-4503-8AFA-7BF4A8443261}" name="Generation Formula"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{EE55000C-7C66-4C54-9EFC-4545134C3C2E}" name="Table8" displayName="Table8" ref="A68:D73" totalsRowShown="0" tableBorderDxfId="4">
-  <autoFilter ref="A68:D73" xr:uid="{EE55000C-7C66-4C54-9EFC-4545134C3C2E}"/>
-  <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{6A5C6F25-06DA-4CE7-AA25-C94719FA66FC}" name="Field" dataDxfId="3"/>
-    <tableColumn id="2" xr3:uid="{FF14DFA8-0D77-4B3A-AE23-8A0B8198D290}" name="Updated Method" dataDxfId="2"/>
-    <tableColumn id="3" xr3:uid="{691D9D89-EEA1-4ACC-A39F-ACEB6C2F9EE5}" name="Storage Method" dataDxfId="1"/>
-    <tableColumn id="4" xr3:uid="{44AC8C37-7AC7-46E0-912B-480A0A44FB88}" name="Datatype" dataDxfId="0"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{EE55000C-7C66-4C54-9EFC-4545134C3C2E}" name="Table8" displayName="Table8" ref="A69:E75" totalsRowShown="0" tableBorderDxfId="6">
+  <autoFilter ref="A69:E75" xr:uid="{EE55000C-7C66-4C54-9EFC-4545134C3C2E}"/>
+  <tableColumns count="5">
+    <tableColumn id="1" xr3:uid="{6A5C6F25-06DA-4CE7-AA25-C94719FA66FC}" name="Field" dataDxfId="5"/>
+    <tableColumn id="2" xr3:uid="{FF14DFA8-0D77-4B3A-AE23-8A0B8198D290}" name="Updated Method" dataDxfId="4"/>
+    <tableColumn id="3" xr3:uid="{691D9D89-EEA1-4ACC-A39F-ACEB6C2F9EE5}" name="Storage Method" dataDxfId="3"/>
+    <tableColumn id="4" xr3:uid="{44AC8C37-7AC7-46E0-912B-480A0A44FB88}" name="Datatype" dataDxfId="2"/>
+    <tableColumn id="5" xr3:uid="{CF6D762C-1B49-4050-9518-2ED8267DAFCA}" name="Generation Formula" dataDxfId="1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1115,24 +1270,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3EF971A8-AD54-4406-A028-7A2295393BC1}">
-  <dimension ref="A1:D73"/>
+  <dimension ref="A1:E75"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" activeCellId="3" sqref="A1:A1048576 B1:B1048576 C1:C1048576 D1:D1048576"/>
+    <sheetView tabSelected="1" topLeftCell="A56" workbookViewId="0">
+      <selection activeCell="C78" sqref="C78"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="31.54296875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="34.26953125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="36.6328125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="32.7265625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10.81640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="32.7265625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="64.08984375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" s="6" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.35">
@@ -1300,7 +1455,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>35</v>
       </c>
@@ -1311,7 +1466,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>36</v>
       </c>
@@ -1322,7 +1477,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>37</v>
       </c>
@@ -1333,7 +1488,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>38</v>
       </c>
@@ -1344,7 +1499,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>39</v>
       </c>
@@ -1355,7 +1510,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>40</v>
       </c>
@@ -1366,7 +1521,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>41</v>
       </c>
@@ -1377,12 +1532,12 @@
         <v>46</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A25" s="6" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>49</v>
       </c>
@@ -1395,8 +1550,11 @@
       <c r="D26" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E26" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>51</v>
       </c>
@@ -1409,8 +1567,11 @@
       <c r="D27" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E27" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>54</v>
       </c>
@@ -1423,8 +1584,11 @@
       <c r="D28" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E28" s="14" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>55</v>
       </c>
@@ -1437,13 +1601,16 @@
       <c r="D29" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E29" s="14" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A31" s="6" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
         <v>49</v>
       </c>
@@ -1456,8 +1623,11 @@
       <c r="D32" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E32" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
         <v>60</v>
       </c>
@@ -1470,8 +1640,11 @@
       <c r="D33" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E33" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
         <v>61</v>
       </c>
@@ -1484,8 +1657,11 @@
       <c r="D34" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E34" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
         <v>62</v>
       </c>
@@ -1498,8 +1674,11 @@
       <c r="D35" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E35" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A36" s="7" t="s">
         <v>54</v>
       </c>
@@ -1512,8 +1691,11 @@
       <c r="D36" s="9" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E36" s="14" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A37" s="7" t="s">
         <v>55</v>
       </c>
@@ -1526,13 +1708,16 @@
       <c r="D37" s="9" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E37" s="14" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A39" s="6" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
         <v>49</v>
       </c>
@@ -1545,8 +1730,11 @@
       <c r="D40" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E40" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
         <v>64</v>
       </c>
@@ -1559,8 +1747,9 @@
       <c r="D41" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E41" s="16"/>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
         <v>65</v>
       </c>
@@ -1573,8 +1762,9 @@
       <c r="D42" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E42" s="16"/>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
         <v>66</v>
       </c>
@@ -1587,8 +1777,9 @@
       <c r="D43" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E43" s="16"/>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
         <v>67</v>
       </c>
@@ -1601,8 +1792,9 @@
       <c r="D44" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E44" s="16"/>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A45" s="7" t="s">
         <v>54</v>
       </c>
@@ -1615,8 +1807,9 @@
       <c r="D45" s="9" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E45" s="17"/>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A46" s="7" t="s">
         <v>55</v>
       </c>
@@ -1629,13 +1822,14 @@
       <c r="D46" s="9" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E46" s="17"/>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A48" s="6" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
         <v>49</v>
       </c>
@@ -1648,8 +1842,11 @@
       <c r="D49" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E49" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
         <v>64</v>
       </c>
@@ -1662,8 +1859,11 @@
       <c r="D50" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E50" s="14" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A51" s="7" t="s">
         <v>65</v>
       </c>
@@ -1676,8 +1876,9 @@
       <c r="D51" s="9" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E51" s="18"/>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A52" s="7" t="s">
         <v>66</v>
       </c>
@@ -1690,8 +1891,9 @@
       <c r="D52" s="9" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E52" s="19"/>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A53" t="s">
         <v>69</v>
       </c>
@@ -1704,8 +1906,9 @@
       <c r="D53" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E53" s="19"/>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A54" t="s">
         <v>70</v>
       </c>
@@ -1718,8 +1921,11 @@
       <c r="D54" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E54" s="14" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A55" s="7" t="s">
         <v>54</v>
       </c>
@@ -1732,8 +1938,11 @@
       <c r="D55" s="9" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E55" s="14" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A56" s="7" t="s">
         <v>55</v>
       </c>
@@ -1746,13 +1955,16 @@
       <c r="D56" s="9" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E56" s="14" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A58" s="6" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A59" t="s">
         <v>49</v>
       </c>
@@ -1765,8 +1977,11 @@
       <c r="D59" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E59" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A60" t="s">
         <v>73</v>
       </c>
@@ -1779,8 +1994,11 @@
       <c r="D60" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E60" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A61" t="s">
         <v>74</v>
       </c>
@@ -1793,8 +2011,11 @@
       <c r="D61" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E61" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A62" t="s">
         <v>75</v>
       </c>
@@ -1807,8 +2028,11 @@
       <c r="D62" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E62" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A63" s="7" t="s">
         <v>54</v>
       </c>
@@ -1821,8 +2045,11 @@
       <c r="D63" s="9" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E63" s="14" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A64" s="10" t="s">
         <v>55</v>
       </c>
@@ -1835,108 +2062,164 @@
       <c r="D64" s="12" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A65" t="s">
-        <v>76</v>
-      </c>
-      <c r="B65" t="s">
-        <v>42</v>
-      </c>
-      <c r="C65" t="s">
-        <v>53</v>
-      </c>
-      <c r="D65" t="s">
+      <c r="E64" s="14" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A65" s="13" t="s">
+        <v>88</v>
+      </c>
+      <c r="B65" s="13" t="s">
+        <v>42</v>
+      </c>
+      <c r="C65" s="13" t="s">
+        <v>53</v>
+      </c>
+      <c r="D65" s="13" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A67" s="6" t="s">
+      <c r="E65" s="15" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A66" t="s">
+        <v>89</v>
+      </c>
+      <c r="B66" t="s">
+        <v>42</v>
+      </c>
+      <c r="C66" t="s">
+        <v>53</v>
+      </c>
+      <c r="D66" t="s">
+        <v>56</v>
+      </c>
+      <c r="E66" s="16"/>
+    </row>
+    <row r="68" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A68" s="6" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A68" t="s">
+    <row r="69" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A69" t="s">
         <v>49</v>
       </c>
-      <c r="B68" t="s">
+      <c r="B69" t="s">
         <v>43</v>
       </c>
-      <c r="C68" t="s">
+      <c r="C69" t="s">
         <v>47</v>
       </c>
-      <c r="D68" t="s">
+      <c r="D69" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A69" t="s">
+      <c r="E69" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A70" t="s">
         <v>64</v>
       </c>
-      <c r="B69" t="s">
-        <v>42</v>
-      </c>
-      <c r="C69" t="s">
-        <v>53</v>
-      </c>
-      <c r="D69" t="s">
+      <c r="B70" t="s">
+        <v>42</v>
+      </c>
+      <c r="C70" t="s">
+        <v>53</v>
+      </c>
+      <c r="D70" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A70" s="7" t="s">
+      <c r="E70" s="14" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A71" t="s">
+        <v>27</v>
+      </c>
+      <c r="B71" t="s">
+        <v>42</v>
+      </c>
+      <c r="C71" t="s">
+        <v>53</v>
+      </c>
+      <c r="D71" t="s">
+        <v>56</v>
+      </c>
+      <c r="E71" s="14" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A72" s="7" t="s">
         <v>65</v>
       </c>
-      <c r="B70" s="8" t="s">
-        <v>42</v>
-      </c>
-      <c r="C70" s="8" t="s">
-        <v>53</v>
-      </c>
-      <c r="D70" s="9" t="s">
+      <c r="B72" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="C72" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="D72" s="9" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A71" s="7" t="s">
+      <c r="E72" s="14" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A73" s="7" t="s">
         <v>66</v>
       </c>
-      <c r="B71" s="8" t="s">
-        <v>42</v>
-      </c>
-      <c r="C71" s="8" t="s">
-        <v>53</v>
-      </c>
-      <c r="D71" s="9" t="s">
+      <c r="B73" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="C73" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="D73" s="9" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A72" s="7" t="s">
+      <c r="E73" s="14" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A74" s="7" t="s">
         <v>54</v>
       </c>
-      <c r="B72" s="8" t="s">
-        <v>42</v>
-      </c>
-      <c r="C72" s="8" t="s">
-        <v>53</v>
-      </c>
-      <c r="D72" s="9" t="s">
+      <c r="B74" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="C74" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="D74" s="9" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A73" s="7" t="s">
+      <c r="E74" s="14" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A75" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="B73" s="8" t="s">
+      <c r="B75" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="C73" s="8" t="s">
+      <c r="C75" s="8" t="s">
         <v>48</v>
       </c>
-      <c r="D73" s="9" t="s">
+      <c r="D75" s="9" t="s">
         <v>57</v>
+      </c>
+      <c r="E75" s="14" t="s">
+        <v>83</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added formulaes for PL Dashboard
</commit_message>
<xml_diff>
--- a/Endpoints.xlsx
+++ b/Endpoints.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Environment\DEV\Documentation\stock-project-documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{334452F8-040B-4C5F-B535-B0D6D4FEA6BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AFAB502E-2D7B-436D-9599-460A415653D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{30700010-F763-4196-BFD8-63DDF9783492}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="319" uniqueCount="127">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="326" uniqueCount="132">
   <si>
     <t>Class</t>
   </si>
@@ -239,27 +239,12 @@
     <t>Fetch from db</t>
   </si>
   <si>
-    <t>sum(sellPrice) - sum(buyPrice)  from profit-loss table</t>
-  </si>
-  <si>
-    <t>sum(buyPrice)  from profit-loss table</t>
-  </si>
-  <si>
-    <t>sum(sellPrice)  from profit-loss table</t>
-  </si>
-  <si>
-    <t>latest(investmentDate) from profit-loss table</t>
-  </si>
-  <si>
     <t xml:space="preserve">Average Return Per Transaction </t>
   </si>
   <si>
     <t>Average Return Percent Per Transaction</t>
   </si>
   <si>
-    <t>(overall p/l - overall bought)/count(records) from profit-loss table</t>
-  </si>
-  <si>
     <t>sum(amountAdded) from mutual-fund table</t>
   </si>
   <si>
@@ -428,13 +413,43 @@
     <t>sum(regularMarketPrice * quantity)  from individual stock API's response</t>
   </si>
   <si>
-    <t>Stock Current Return * 100 / Stock Current Value</t>
-  </si>
-  <si>
     <t>latest(investment_date) from stock table</t>
   </si>
   <si>
     <t>Fetch from dB(select stock_updated_date from miscellaneous_record)</t>
+  </si>
+  <si>
+    <t>Stock Current Return * 100 / Stock Investment Value</t>
+  </si>
+  <si>
+    <t>Overall P/L /count(records) from profit-loss table</t>
+  </si>
+  <si>
+    <t>Overall P/L Percent</t>
+  </si>
+  <si>
+    <t>(Overall P/L * 100)/Overall Bought Amount from profit-loss table</t>
+  </si>
+  <si>
+    <t>sum(ReturnPercent(buy_price,sell_price))/count(records)</t>
+  </si>
+  <si>
+    <t>sum(sell_price) - sum(buy_price)  from profit-loss table</t>
+  </si>
+  <si>
+    <t>sum(buy_price)  from profit-loss table</t>
+  </si>
+  <si>
+    <t>sum(sell_price)  from profit-loss table</t>
+  </si>
+  <si>
+    <t>latest(investment_date) from profit-loss table</t>
+  </si>
+  <si>
+    <t>Fetch from dB(select profit_loss_updated_date from miscellaneous_record)</t>
+  </si>
+  <si>
+    <t>"/profit-loss-dashboard" API</t>
   </si>
 </sst>
 </file>
@@ -638,7 +653,7 @@
     <xf numFmtId="0" fontId="4" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -676,6 +691,7 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="4"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="8">
     <cellStyle name="60% - Accent4" xfId="6" builtinId="44"/>
@@ -710,9 +726,19 @@
         <right style="thin">
           <color theme="4"/>
         </right>
-        <top style="thin">
+        <top/>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="thin">
           <color theme="4"/>
-        </top>
+        </right>
+        <top/>
         <bottom/>
         <vertical/>
         <horizontal/>
@@ -839,20 +865,6 @@
         <bottom style="thin">
           <color theme="4"/>
         </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right style="thin">
-          <color theme="4"/>
-        </right>
-        <top style="thin">
-          <color theme="4"/>
-        </top>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
       </border>
     </dxf>
     <dxf>
@@ -1012,8 +1024,8 @@
     <tableColumn id="1" xr3:uid="{688E3C3B-D317-4C98-A054-3BE5422EA63F}" name="Field"/>
     <tableColumn id="2" xr3:uid="{B511B556-A733-4517-8C85-34070BFC361B}" name="Updated Method"/>
     <tableColumn id="3" xr3:uid="{59E920CB-0533-4CE8-908B-0C7E19004603}" name="Storage Method"/>
+    <tableColumn id="5" xr3:uid="{B7C54223-7E16-496C-BCCF-87B18D195F88}" name="Generation Formula"/>
     <tableColumn id="4" xr3:uid="{06FE7570-AA3C-48D2-8F0A-2E7E00298919}" name="Datatype"/>
-    <tableColumn id="5" xr3:uid="{B7C54223-7E16-496C-BCCF-87B18D195F88}" name="Generation Formula"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1026,8 +1038,8 @@
     <tableColumn id="1" xr3:uid="{4FEFCDF2-FE87-456F-8582-283484542A4C}" name="Field"/>
     <tableColumn id="2" xr3:uid="{E37067D1-9308-49A6-951C-A0E4C1195265}" name="Updated Method"/>
     <tableColumn id="3" xr3:uid="{A870BFD7-27F4-40E5-A72B-A4CC431BE64F}" name="Storage Method"/>
+    <tableColumn id="5" xr3:uid="{0A1B7B91-9E94-4EE5-B841-DB66A0475DDB}" name="Generation Formula"/>
     <tableColumn id="4" xr3:uid="{CC68BEF1-5A7D-4E13-80F5-40174E39F5A1}" name="Datatype"/>
-    <tableColumn id="5" xr3:uid="{0A1B7B91-9E94-4EE5-B841-DB66A0475DDB}" name="Generation Formula"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1040,8 +1052,8 @@
     <tableColumn id="1" xr3:uid="{EBB6A018-4229-44E2-BFEC-5735124A49D6}" name="Field"/>
     <tableColumn id="2" xr3:uid="{FC54E304-E834-423E-9BAD-E6E45489B546}" name="Updated Method"/>
     <tableColumn id="3" xr3:uid="{613DDB66-D41E-4B6C-B527-E8DFC784E985}" name="Storage Method"/>
+    <tableColumn id="5" xr3:uid="{A64F5098-7655-48F5-AF7E-F022BCE52994}" name="Generation Formula" dataCellStyle="Accent3"/>
     <tableColumn id="4" xr3:uid="{9C6A3024-B511-49C3-B5CC-FCFDE9C75704}" name="Datatype"/>
-    <tableColumn id="5" xr3:uid="{A64F5098-7655-48F5-AF7E-F022BCE52994}" name="Generation Formula" dataCellStyle="Accent3"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1054,36 +1066,36 @@
     <tableColumn id="1" xr3:uid="{A46E78D4-40E3-4CC2-9E07-4DABCC13ECD1}" name="Field" dataDxfId="10"/>
     <tableColumn id="2" xr3:uid="{8A2E0C0E-C378-49DE-BA9B-6CA0CCEAFBF3}" name="Updated Method" dataDxfId="9"/>
     <tableColumn id="3" xr3:uid="{63A090DB-A088-4A75-AB57-104DB398EB6A}" name="Storage Method" dataDxfId="8"/>
+    <tableColumn id="5" xr3:uid="{DB5D1536-7619-490E-9FE4-86DA2FB10366}" name="Generation Formula" dataDxfId="1" dataCellStyle="Accent3"/>
     <tableColumn id="4" xr3:uid="{DAC83841-7394-440C-B6AC-A9D73F43D271}" name="Datatype" dataDxfId="7"/>
-    <tableColumn id="5" xr3:uid="{DB5D1536-7619-490E-9FE4-86DA2FB10366}" name="Generation Formula" dataDxfId="6" dataCellStyle="Accent3"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{7E2565EE-2AC7-45FA-8DCC-4FA501A0CBAE}" name="Table7" displayName="Table7" ref="A59:E66" totalsRowShown="0">
-  <autoFilter ref="A59:E66" xr:uid="{7E2565EE-2AC7-45FA-8DCC-4FA501A0CBAE}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{7E2565EE-2AC7-45FA-8DCC-4FA501A0CBAE}" name="Table7" displayName="Table7" ref="A59:E67" totalsRowShown="0">
+  <autoFilter ref="A59:E67" xr:uid="{7E2565EE-2AC7-45FA-8DCC-4FA501A0CBAE}"/>
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{C2B1F201-E24C-4440-A910-1D2DA6518B24}" name="Field"/>
     <tableColumn id="2" xr3:uid="{24B8A508-38BE-4BFD-A43A-7033CE93F7DF}" name="Updated Method"/>
     <tableColumn id="3" xr3:uid="{9A831C7C-F95F-4CE5-A352-41936EE80EEC}" name="Storage Method"/>
+    <tableColumn id="5" xr3:uid="{593FFB5A-2ED0-4503-8AFA-7BF4A8443261}" name="Generation Formula"/>
     <tableColumn id="4" xr3:uid="{2D5D09E6-B72E-47AC-92C5-4AE0287C67FB}" name="Datatype"/>
-    <tableColumn id="5" xr3:uid="{593FFB5A-2ED0-4503-8AFA-7BF4A8443261}" name="Generation Formula"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{EE55000C-7C66-4C54-9EFC-4545134C3C2E}" name="Table8" displayName="Table8" ref="A69:E75" totalsRowShown="0" tableBorderDxfId="5">
-  <autoFilter ref="A69:E75" xr:uid="{EE55000C-7C66-4C54-9EFC-4545134C3C2E}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{EE55000C-7C66-4C54-9EFC-4545134C3C2E}" name="Table8" displayName="Table8" ref="A70:E76" totalsRowShown="0" tableBorderDxfId="6">
+  <autoFilter ref="A70:E76" xr:uid="{EE55000C-7C66-4C54-9EFC-4545134C3C2E}"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{6A5C6F25-06DA-4CE7-AA25-C94719FA66FC}" name="Field" dataDxfId="4"/>
-    <tableColumn id="2" xr3:uid="{FF14DFA8-0D77-4B3A-AE23-8A0B8198D290}" name="Updated Method" dataDxfId="3"/>
-    <tableColumn id="3" xr3:uid="{691D9D89-EEA1-4ACC-A39F-ACEB6C2F9EE5}" name="Storage Method" dataDxfId="2"/>
-    <tableColumn id="4" xr3:uid="{44AC8C37-7AC7-46E0-912B-480A0A44FB88}" name="Datatype" dataDxfId="1"/>
+    <tableColumn id="1" xr3:uid="{6A5C6F25-06DA-4CE7-AA25-C94719FA66FC}" name="Field" dataDxfId="5"/>
+    <tableColumn id="2" xr3:uid="{FF14DFA8-0D77-4B3A-AE23-8A0B8198D290}" name="Updated Method" dataDxfId="4"/>
+    <tableColumn id="3" xr3:uid="{691D9D89-EEA1-4ACC-A39F-ACEB6C2F9EE5}" name="Storage Method" dataDxfId="3"/>
     <tableColumn id="5" xr3:uid="{CF6D762C-1B49-4050-9518-2ED8267DAFCA}" name="Generation Formula" dataDxfId="0"/>
+    <tableColumn id="4" xr3:uid="{44AC8C37-7AC7-46E0-912B-480A0A44FB88}" name="Datatype" dataDxfId="2"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1399,10 +1411,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3EF971A8-AD54-4406-A028-7A2295393BC1}">
-  <dimension ref="A1:E75"/>
+  <dimension ref="A1:E76"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A65" workbookViewId="0">
-      <selection activeCell="A68" sqref="A68"/>
+    <sheetView tabSelected="1" topLeftCell="A66" workbookViewId="0">
+      <selection activeCell="D58" sqref="D58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1444,12 +1456,12 @@
         <v>32</v>
       </c>
       <c r="D3" s="19" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4" s="18" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="B4" s="18" t="s">
         <v>27</v>
@@ -1458,7 +1470,7 @@
         <v>30</v>
       </c>
       <c r="D4" s="18" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.35">
@@ -1472,12 +1484,12 @@
         <v>30</v>
       </c>
       <c r="D5" s="18" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A6" s="18" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="B6" s="18" t="s">
         <v>27</v>
@@ -1486,7 +1498,7 @@
         <v>30</v>
       </c>
       <c r="D6" s="18" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.35">
@@ -1500,12 +1512,12 @@
         <v>30</v>
       </c>
       <c r="D7" s="18" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A8" s="19" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="B8" s="19" t="s">
         <v>27</v>
@@ -1514,12 +1526,12 @@
         <v>30</v>
       </c>
       <c r="D8" s="20" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A9" s="19" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="B9" s="19" t="s">
         <v>27</v>
@@ -1528,12 +1540,12 @@
         <v>30</v>
       </c>
       <c r="D9" s="20" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A10" s="19" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="B10" s="19" t="s">
         <v>27</v>
@@ -1542,12 +1554,12 @@
         <v>30</v>
       </c>
       <c r="D10" s="19" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A11" s="19" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="B11" s="19" t="s">
         <v>27</v>
@@ -1556,54 +1568,54 @@
         <v>30</v>
       </c>
       <c r="D11" s="19" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A12" s="18" t="s">
+        <v>85</v>
+      </c>
+      <c r="B12" s="18" t="s">
+        <v>27</v>
+      </c>
+      <c r="C12" s="18" t="s">
+        <v>30</v>
+      </c>
+      <c r="D12" s="22" t="s">
         <v>90</v>
-      </c>
-      <c r="B12" s="18" t="s">
-        <v>27</v>
-      </c>
-      <c r="C12" s="18" t="s">
-        <v>30</v>
-      </c>
-      <c r="D12" s="22" t="s">
-        <v>95</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A13" s="18" t="s">
+        <v>86</v>
+      </c>
+      <c r="B13" s="18" t="s">
+        <v>27</v>
+      </c>
+      <c r="C13" s="18" t="s">
+        <v>30</v>
+      </c>
+      <c r="D13" s="22" t="s">
         <v>91</v>
-      </c>
-      <c r="B13" s="18" t="s">
-        <v>27</v>
-      </c>
-      <c r="C13" s="18" t="s">
-        <v>30</v>
-      </c>
-      <c r="D13" s="22" t="s">
-        <v>96</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A14" s="18" t="s">
+        <v>87</v>
+      </c>
+      <c r="B14" s="18" t="s">
+        <v>27</v>
+      </c>
+      <c r="C14" s="18" t="s">
+        <v>30</v>
+      </c>
+      <c r="D14" s="18" t="s">
         <v>92</v>
-      </c>
-      <c r="B14" s="18" t="s">
-        <v>27</v>
-      </c>
-      <c r="C14" s="18" t="s">
-        <v>30</v>
-      </c>
-      <c r="D14" s="18" t="s">
-        <v>97</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A15" s="18" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="B15" s="18" t="s">
         <v>27</v>
@@ -1612,12 +1624,12 @@
         <v>30</v>
       </c>
       <c r="D15" s="18" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A16" s="19" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="B16" s="19" t="s">
         <v>27</v>
@@ -1626,12 +1638,12 @@
         <v>30</v>
       </c>
       <c r="D16" s="20" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A17" s="19" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="B17" s="19" t="s">
         <v>27</v>
@@ -1640,12 +1652,12 @@
         <v>30</v>
       </c>
       <c r="D17" s="20" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A18" s="19" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="B18" s="19" t="s">
         <v>27</v>
@@ -1654,12 +1666,12 @@
         <v>30</v>
       </c>
       <c r="D18" s="19" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A19" s="19" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="B19" s="19" t="s">
         <v>27</v>
@@ -1668,12 +1680,12 @@
         <v>30</v>
       </c>
       <c r="D19" s="19" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A20" s="18" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="B20" s="18" t="s">
         <v>27</v>
@@ -1682,12 +1694,12 @@
         <v>30</v>
       </c>
       <c r="D20" s="22" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A21" s="19" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="B21" s="19" t="s">
         <v>27</v>
@@ -1696,12 +1708,12 @@
         <v>30</v>
       </c>
       <c r="D21" s="20" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A22" s="19" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="B22" s="19" t="s">
         <v>27</v>
@@ -1710,7 +1722,7 @@
         <v>30</v>
       </c>
       <c r="D22" s="19" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.35">
@@ -1724,7 +1736,7 @@
         <v>30</v>
       </c>
       <c r="D23" s="18" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.35">
@@ -1732,7 +1744,7 @@
         <v>34</v>
       </c>
       <c r="B25" s="23" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.35">
@@ -1746,15 +1758,15 @@
         <v>31</v>
       </c>
       <c r="D26" t="s">
+        <v>59</v>
+      </c>
+      <c r="E26" t="s">
         <v>40</v>
-      </c>
-      <c r="E26" t="s">
-        <v>59</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
       <c r="B27" t="s">
         <v>27</v>
@@ -1763,10 +1775,10 @@
         <v>30</v>
       </c>
       <c r="D27" t="s">
+        <v>107</v>
+      </c>
+      <c r="E27" t="s">
         <v>38</v>
-      </c>
-      <c r="E27" t="s">
-        <v>112</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.35">
@@ -1779,11 +1791,11 @@
       <c r="C28" t="s">
         <v>30</v>
       </c>
-      <c r="D28" t="s">
+      <c r="D28" s="13" t="s">
+        <v>108</v>
+      </c>
+      <c r="E28" t="s">
         <v>39</v>
-      </c>
-      <c r="E28" s="13" t="s">
-        <v>113</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.35">
@@ -1796,11 +1808,11 @@
       <c r="C29" t="s">
         <v>32</v>
       </c>
-      <c r="D29" t="s">
+      <c r="D29" s="13" t="s">
+        <v>109</v>
+      </c>
+      <c r="E29" t="s">
         <v>39</v>
-      </c>
-      <c r="E29" s="13" t="s">
-        <v>114</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.35">
@@ -1808,7 +1820,7 @@
         <v>41</v>
       </c>
       <c r="B31" s="23" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.35">
@@ -1822,10 +1834,10 @@
         <v>31</v>
       </c>
       <c r="D32" t="s">
+        <v>59</v>
+      </c>
+      <c r="E32" t="s">
         <v>40</v>
-      </c>
-      <c r="E32" t="s">
-        <v>59</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.35">
@@ -1839,10 +1851,10 @@
         <v>30</v>
       </c>
       <c r="D33" t="s">
+        <v>110</v>
+      </c>
+      <c r="E33" t="s">
         <v>38</v>
-      </c>
-      <c r="E33" t="s">
-        <v>115</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.35">
@@ -1856,10 +1868,10 @@
         <v>30</v>
       </c>
       <c r="D34" t="s">
+        <v>111</v>
+      </c>
+      <c r="E34" t="s">
         <v>38</v>
-      </c>
-      <c r="E34" t="s">
-        <v>116</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.35">
@@ -1873,10 +1885,10 @@
         <v>30</v>
       </c>
       <c r="D35" t="s">
+        <v>112</v>
+      </c>
+      <c r="E35" t="s">
         <v>38</v>
-      </c>
-      <c r="E35" t="s">
-        <v>117</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.35">
@@ -1889,11 +1901,11 @@
       <c r="C36" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="D36" s="9" t="s">
+      <c r="D36" s="13" t="s">
+        <v>113</v>
+      </c>
+      <c r="E36" s="9" t="s">
         <v>39</v>
-      </c>
-      <c r="E36" s="13" t="s">
-        <v>118</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.35">
@@ -1906,11 +1918,11 @@
       <c r="C37" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="D37" s="9" t="s">
+      <c r="D37" s="13" t="s">
+        <v>114</v>
+      </c>
+      <c r="E37" s="9" t="s">
         <v>39</v>
-      </c>
-      <c r="E37" s="13" t="s">
-        <v>119</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.35">
@@ -1929,10 +1941,10 @@
         <v>31</v>
       </c>
       <c r="D40" t="s">
+        <v>59</v>
+      </c>
+      <c r="E40" t="s">
         <v>40</v>
-      </c>
-      <c r="E40" t="s">
-        <v>59</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.35">
@@ -1945,10 +1957,10 @@
       <c r="C41" t="s">
         <v>35</v>
       </c>
-      <c r="D41" t="s">
+      <c r="D41" s="14"/>
+      <c r="E41" t="s">
         <v>38</v>
       </c>
-      <c r="E41" s="14"/>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
@@ -1960,10 +1972,10 @@
       <c r="C42" t="s">
         <v>35</v>
       </c>
-      <c r="D42" t="s">
+      <c r="D42" s="14"/>
+      <c r="E42" t="s">
         <v>38</v>
       </c>
-      <c r="E42" s="14"/>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
@@ -1975,10 +1987,10 @@
       <c r="C43" t="s">
         <v>35</v>
       </c>
-      <c r="D43" t="s">
+      <c r="D43" s="14"/>
+      <c r="E43" t="s">
         <v>38</v>
       </c>
-      <c r="E43" s="14"/>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
@@ -1990,10 +2002,10 @@
       <c r="C44" t="s">
         <v>35</v>
       </c>
-      <c r="D44" t="s">
+      <c r="D44" s="14"/>
+      <c r="E44" t="s">
         <v>38</v>
       </c>
-      <c r="E44" s="14"/>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A45" s="7" t="s">
@@ -2005,10 +2017,10 @@
       <c r="C45" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="D45" s="9" t="s">
+      <c r="D45" s="15"/>
+      <c r="E45" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="E45" s="15"/>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A46" s="7" t="s">
@@ -2020,10 +2032,10 @@
       <c r="C46" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="D46" s="9" t="s">
+      <c r="D46" s="15"/>
+      <c r="E46" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="E46" s="15"/>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A48" s="21" t="s">
@@ -2041,10 +2053,10 @@
         <v>31</v>
       </c>
       <c r="D49" t="s">
+        <v>59</v>
+      </c>
+      <c r="E49" t="s">
         <v>40</v>
-      </c>
-      <c r="E49" t="s">
-        <v>59</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.35">
@@ -2057,11 +2069,11 @@
       <c r="C50" t="s">
         <v>35</v>
       </c>
-      <c r="D50" t="s">
+      <c r="D50" s="17" t="s">
+        <v>63</v>
+      </c>
+      <c r="E50" t="s">
         <v>38</v>
-      </c>
-      <c r="E50" s="17" t="s">
-        <v>68</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.35">
@@ -2074,10 +2086,10 @@
       <c r="C51" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="D51" s="9" t="s">
+      <c r="D51" s="16"/>
+      <c r="E51" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="E51" s="16"/>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A52" s="7" t="s">
@@ -2089,10 +2101,10 @@
       <c r="C52" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="D52" s="9" t="s">
+      <c r="D52" s="17"/>
+      <c r="E52" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="E52" s="17"/>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A53" t="s">
@@ -2104,10 +2116,10 @@
       <c r="C53" t="s">
         <v>35</v>
       </c>
-      <c r="D53" t="s">
+      <c r="D53" s="17"/>
+      <c r="E53" t="s">
         <v>38</v>
       </c>
-      <c r="E53" s="17"/>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A54" t="s">
@@ -2119,11 +2131,11 @@
       <c r="C54" t="s">
         <v>35</v>
       </c>
-      <c r="D54" t="s">
+      <c r="D54" s="17" t="s">
+        <v>64</v>
+      </c>
+      <c r="E54" t="s">
         <v>38</v>
-      </c>
-      <c r="E54" s="17" t="s">
-        <v>69</v>
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.35">
@@ -2136,11 +2148,11 @@
       <c r="C55" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="D55" s="9" t="s">
+      <c r="D55" s="17" t="s">
+        <v>65</v>
+      </c>
+      <c r="E55" s="9" t="s">
         <v>39</v>
-      </c>
-      <c r="E55" s="17" t="s">
-        <v>70</v>
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.35">
@@ -2153,16 +2165,19 @@
       <c r="C56" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="D56" s="9" t="s">
+      <c r="D56" s="17" t="s">
+        <v>60</v>
+      </c>
+      <c r="E56" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="E56" s="17" t="s">
-        <v>60</v>
-      </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A58" s="21" t="s">
+      <c r="A58" s="24" t="s">
         <v>54</v>
+      </c>
+      <c r="B58" t="s">
+        <v>131</v>
       </c>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.35">
@@ -2176,10 +2191,10 @@
         <v>31</v>
       </c>
       <c r="D59" t="s">
+        <v>59</v>
+      </c>
+      <c r="E59" t="s">
         <v>40</v>
-      </c>
-      <c r="E59" t="s">
-        <v>59</v>
       </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.35">
@@ -2190,13 +2205,13 @@
         <v>27</v>
       </c>
       <c r="C60" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="D60" t="s">
+        <v>126</v>
+      </c>
+      <c r="E60" t="s">
         <v>38</v>
-      </c>
-      <c r="E60" t="s">
-        <v>61</v>
       </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.35">
@@ -2207,13 +2222,13 @@
         <v>27</v>
       </c>
       <c r="C61" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="D61" t="s">
+        <v>127</v>
+      </c>
+      <c r="E61" t="s">
         <v>38</v>
-      </c>
-      <c r="E61" t="s">
-        <v>62</v>
       </c>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.35">
@@ -2224,13 +2239,13 @@
         <v>27</v>
       </c>
       <c r="C62" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="D62" t="s">
+        <v>128</v>
+      </c>
+      <c r="E62" t="s">
         <v>38</v>
-      </c>
-      <c r="E62" t="s">
-        <v>63</v>
       </c>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.35">
@@ -2241,13 +2256,13 @@
         <v>27</v>
       </c>
       <c r="C63" s="8" t="s">
-        <v>35</v>
-      </c>
-      <c r="D63" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="D63" s="13" t="s">
+        <v>129</v>
+      </c>
+      <c r="E63" s="9" t="s">
         <v>39</v>
-      </c>
-      <c r="E63" s="13" t="s">
-        <v>64</v>
       </c>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.35">
@@ -2260,90 +2275,92 @@
       <c r="C64" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="D64" s="12" t="s">
+      <c r="D64" s="13" t="s">
+        <v>130</v>
+      </c>
+      <c r="E64" s="12" t="s">
         <v>39</v>
       </c>
-      <c r="E64" s="13" t="s">
-        <v>60</v>
-      </c>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A65" t="s">
-        <v>65</v>
-      </c>
-      <c r="B65" t="s">
-        <v>27</v>
-      </c>
-      <c r="C65" t="s">
-        <v>35</v>
-      </c>
-      <c r="D65" t="s">
+      <c r="A65" s="25" t="s">
+        <v>123</v>
+      </c>
+      <c r="B65" s="25" t="s">
+        <v>27</v>
+      </c>
+      <c r="C65" s="25" t="s">
+        <v>30</v>
+      </c>
+      <c r="D65" s="25" t="s">
+        <v>124</v>
+      </c>
+      <c r="E65" s="25" t="s">
         <v>38</v>
-      </c>
-      <c r="E65" s="14" t="s">
-        <v>67</v>
       </c>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A66" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="B66" t="s">
         <v>27</v>
       </c>
       <c r="C66" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="D66" t="s">
+        <v>122</v>
+      </c>
+      <c r="E66" t="s">
         <v>38</v>
       </c>
-      <c r="E66" s="14"/>
-    </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A68" s="24" t="s">
+    </row>
+    <row r="67" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A67" t="s">
+        <v>62</v>
+      </c>
+      <c r="B67" t="s">
+        <v>27</v>
+      </c>
+      <c r="C67" t="s">
+        <v>30</v>
+      </c>
+      <c r="D67" t="s">
+        <v>125</v>
+      </c>
+      <c r="E67" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A69" s="24" t="s">
         <v>53</v>
       </c>
-      <c r="B68" s="23" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A69" t="s">
-        <v>33</v>
-      </c>
-      <c r="B69" t="s">
-        <v>28</v>
-      </c>
-      <c r="C69" t="s">
-        <v>31</v>
-      </c>
-      <c r="D69" t="s">
-        <v>40</v>
-      </c>
-      <c r="E69" t="s">
-        <v>59</v>
+      <c r="B69" s="23" t="s">
+        <v>117</v>
       </c>
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A70" t="s">
-        <v>82</v>
+        <v>33</v>
       </c>
       <c r="B70" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C70" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="D70" t="s">
-        <v>38</v>
-      </c>
-      <c r="E70" s="13" t="s">
-        <v>72</v>
+        <v>59</v>
+      </c>
+      <c r="E70" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A71" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="B71" t="s">
         <v>27</v>
@@ -2351,33 +2368,33 @@
       <c r="C71" t="s">
         <v>30</v>
       </c>
-      <c r="D71" t="s">
+      <c r="D71" s="13" t="s">
+        <v>67</v>
+      </c>
+      <c r="E71" t="s">
         <v>38</v>
       </c>
-      <c r="E71" s="13" t="s">
-        <v>123</v>
-      </c>
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A72" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="B72" s="8" t="s">
+      <c r="A72" t="s">
+        <v>78</v>
+      </c>
+      <c r="B72" t="s">
         <v>27</v>
       </c>
       <c r="C72" t="s">
         <v>30</v>
       </c>
-      <c r="D72" s="9" t="s">
+      <c r="D72" s="13" t="s">
+        <v>118</v>
+      </c>
+      <c r="E72" t="s">
         <v>38</v>
-      </c>
-      <c r="E72" s="13" t="s">
-        <v>78</v>
       </c>
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A73" s="7" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B73" s="8" t="s">
         <v>27</v>
@@ -2385,16 +2402,16 @@
       <c r="C73" t="s">
         <v>30</v>
       </c>
-      <c r="D73" s="9" t="s">
+      <c r="D73" s="13" t="s">
+        <v>73</v>
+      </c>
+      <c r="E73" s="9" t="s">
         <v>38</v>
-      </c>
-      <c r="E73" s="13" t="s">
-        <v>124</v>
       </c>
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A74" s="7" t="s">
-        <v>36</v>
+        <v>26</v>
       </c>
       <c r="B74" s="8" t="s">
         <v>27</v>
@@ -2402,28 +2419,45 @@
       <c r="C74" t="s">
         <v>30</v>
       </c>
-      <c r="D74" s="9" t="s">
-        <v>39</v>
-      </c>
-      <c r="E74" s="13" t="s">
-        <v>125</v>
+      <c r="D74" s="13" t="s">
+        <v>121</v>
+      </c>
+      <c r="E74" s="9" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A75" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="B75" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="C75" t="s">
+        <v>30</v>
+      </c>
+      <c r="D75" s="13" t="s">
+        <v>119</v>
+      </c>
+      <c r="E75" s="9" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A76" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="B75" s="8" t="s">
+      <c r="B76" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="C75" s="8" t="s">
+      <c r="C76" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="D75" s="9" t="s">
+      <c r="D76" s="13" t="s">
+        <v>120</v>
+      </c>
+      <c r="E76" s="9" t="s">
         <v>39</v>
-      </c>
-      <c r="E75" s="13" t="s">
-        <v>126</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added Endpoint for excel upload/Prod data till date
</commit_message>
<xml_diff>
--- a/Endpoints.xlsx
+++ b/Endpoints.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26501"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Environment\DEV\Documentation\stock-project-documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AFAB502E-2D7B-436D-9599-460A415653D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86D97E17-EDEF-4A60-88EA-0247C919C913}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{30700010-F763-4196-BFD8-63DDF9783492}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="326" uniqueCount="132">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="333" uniqueCount="136">
   <si>
     <t>Class</t>
   </si>
@@ -450,6 +450,27 @@
   </si>
   <si>
     <t>"/profit-loss-dashboard" API</t>
+  </si>
+  <si>
+    <t>http://localhost:8080/stock-app/v1/company-dropdowns/with-excel</t>
+  </si>
+  <si>
+    <t>CompanyNameDropdownController</t>
+  </si>
+  <si>
+    <t>{
+     "excelPath":"D:\\StockMarketData\\NSE Companies Data.xlsx",
+     "sheetName":"NSE Companies",
+     "rowStartNumber":1,
+     "columnCharactersToRead":["B","C"]
+}</t>
+  </si>
+  <si>
+    <t>[
+    {
+        "companySymbol": "20MICRONS",
+        "companyName": "20 Microns Limited"
+    },                                                                                                                      ]</t>
   </si>
 </sst>
 </file>
@@ -653,19 +674,10 @@
     <xf numFmtId="0" fontId="4" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -691,7 +703,21 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="4"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="8">
     <cellStyle name="60% - Accent4" xfId="6" builtinId="44"/>
@@ -726,19 +752,9 @@
         <right style="thin">
           <color theme="4"/>
         </right>
-        <top/>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right style="thin">
+        <top style="thin">
           <color theme="4"/>
-        </right>
-        <top/>
+        </top>
         <bottom/>
         <vertical/>
         <horizontal/>
@@ -766,9 +782,7 @@
         <right style="thin">
           <color theme="4"/>
         </right>
-        <top style="thin">
-          <color theme="4"/>
-        </top>
+        <top/>
         <bottom/>
         <vertical/>
         <horizontal/>
@@ -892,6 +906,18 @@
         <top style="thin">
           <color theme="4"/>
         </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="thin">
+          <color theme="4"/>
+        </right>
+        <top/>
         <bottom/>
         <vertical/>
         <horizontal/>
@@ -1066,8 +1092,8 @@
     <tableColumn id="1" xr3:uid="{A46E78D4-40E3-4CC2-9E07-4DABCC13ECD1}" name="Field" dataDxfId="10"/>
     <tableColumn id="2" xr3:uid="{8A2E0C0E-C378-49DE-BA9B-6CA0CCEAFBF3}" name="Updated Method" dataDxfId="9"/>
     <tableColumn id="3" xr3:uid="{63A090DB-A088-4A75-AB57-104DB398EB6A}" name="Storage Method" dataDxfId="8"/>
-    <tableColumn id="5" xr3:uid="{DB5D1536-7619-490E-9FE4-86DA2FB10366}" name="Generation Formula" dataDxfId="1" dataCellStyle="Accent3"/>
-    <tableColumn id="4" xr3:uid="{DAC83841-7394-440C-B6AC-A9D73F43D271}" name="Datatype" dataDxfId="7"/>
+    <tableColumn id="5" xr3:uid="{DB5D1536-7619-490E-9FE4-86DA2FB10366}" name="Generation Formula" dataDxfId="7" dataCellStyle="Accent3"/>
+    <tableColumn id="4" xr3:uid="{DAC83841-7394-440C-B6AC-A9D73F43D271}" name="Datatype" dataDxfId="6"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1088,14 +1114,14 @@
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{EE55000C-7C66-4C54-9EFC-4545134C3C2E}" name="Table8" displayName="Table8" ref="A70:E76" totalsRowShown="0" tableBorderDxfId="6">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{EE55000C-7C66-4C54-9EFC-4545134C3C2E}" name="Table8" displayName="Table8" ref="A70:E76" totalsRowShown="0" tableBorderDxfId="5">
   <autoFilter ref="A70:E76" xr:uid="{EE55000C-7C66-4C54-9EFC-4545134C3C2E}"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{6A5C6F25-06DA-4CE7-AA25-C94719FA66FC}" name="Field" dataDxfId="5"/>
-    <tableColumn id="2" xr3:uid="{FF14DFA8-0D77-4B3A-AE23-8A0B8198D290}" name="Updated Method" dataDxfId="4"/>
-    <tableColumn id="3" xr3:uid="{691D9D89-EEA1-4ACC-A39F-ACEB6C2F9EE5}" name="Storage Method" dataDxfId="3"/>
-    <tableColumn id="5" xr3:uid="{CF6D762C-1B49-4050-9518-2ED8267DAFCA}" name="Generation Formula" dataDxfId="0"/>
-    <tableColumn id="4" xr3:uid="{44AC8C37-7AC7-46E0-912B-480A0A44FB88}" name="Datatype" dataDxfId="2"/>
+    <tableColumn id="1" xr3:uid="{6A5C6F25-06DA-4CE7-AA25-C94719FA66FC}" name="Field" dataDxfId="4"/>
+    <tableColumn id="2" xr3:uid="{FF14DFA8-0D77-4B3A-AE23-8A0B8198D290}" name="Updated Method" dataDxfId="3"/>
+    <tableColumn id="3" xr3:uid="{691D9D89-EEA1-4ACC-A39F-ACEB6C2F9EE5}" name="Storage Method" dataDxfId="2"/>
+    <tableColumn id="5" xr3:uid="{CF6D762C-1B49-4050-9518-2ED8267DAFCA}" name="Generation Formula" dataDxfId="1"/>
+    <tableColumn id="4" xr3:uid="{44AC8C37-7AC7-46E0-912B-480A0A44FB88}" name="Datatype" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1413,7 +1439,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3EF971A8-AD54-4406-A028-7A2295393BC1}">
   <dimension ref="A1:E76"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A66" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="D58" sqref="D58"/>
     </sheetView>
   </sheetViews>
@@ -1427,7 +1453,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="3" t="s">
         <v>58</v>
       </c>
     </row>
@@ -1446,304 +1472,304 @@
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A3" s="19" t="s">
+      <c r="A3" s="16" t="s">
         <v>22</v>
       </c>
-      <c r="B3" s="19" t="s">
+      <c r="B3" s="16" t="s">
         <v>29</v>
       </c>
-      <c r="C3" s="19" t="s">
+      <c r="C3" s="16" t="s">
         <v>32</v>
       </c>
-      <c r="D3" s="19" t="s">
+      <c r="D3" s="16" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A4" s="18" t="s">
+      <c r="A4" s="15" t="s">
         <v>68</v>
       </c>
-      <c r="B4" s="18" t="s">
-        <v>27</v>
-      </c>
-      <c r="C4" s="18" t="s">
-        <v>30</v>
-      </c>
-      <c r="D4" s="18" t="s">
+      <c r="B4" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="C4" s="15" t="s">
+        <v>30</v>
+      </c>
+      <c r="D4" s="15" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A5" s="18" t="s">
+      <c r="A5" s="15" t="s">
         <v>23</v>
       </c>
-      <c r="B5" s="18" t="s">
-        <v>27</v>
-      </c>
-      <c r="C5" s="18" t="s">
-        <v>30</v>
-      </c>
-      <c r="D5" s="18" t="s">
+      <c r="B5" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="C5" s="15" t="s">
+        <v>30</v>
+      </c>
+      <c r="D5" s="15" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A6" s="18" t="s">
+      <c r="A6" s="15" t="s">
         <v>71</v>
       </c>
-      <c r="B6" s="18" t="s">
-        <v>27</v>
-      </c>
-      <c r="C6" s="18" t="s">
-        <v>30</v>
-      </c>
-      <c r="D6" s="18" t="s">
+      <c r="B6" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="C6" s="15" t="s">
+        <v>30</v>
+      </c>
+      <c r="D6" s="15" t="s">
         <v>72</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A7" s="18" t="s">
+      <c r="A7" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="B7" s="18" t="s">
-        <v>27</v>
-      </c>
-      <c r="C7" s="18" t="s">
-        <v>30</v>
-      </c>
-      <c r="D7" s="18" t="s">
+      <c r="B7" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="C7" s="15" t="s">
+        <v>30</v>
+      </c>
+      <c r="D7" s="15" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A8" s="19" t="s">
+      <c r="A8" s="16" t="s">
         <v>77</v>
       </c>
-      <c r="B8" s="19" t="s">
-        <v>27</v>
-      </c>
-      <c r="C8" s="19" t="s">
-        <v>30</v>
-      </c>
-      <c r="D8" s="20" t="s">
+      <c r="B8" s="16" t="s">
+        <v>27</v>
+      </c>
+      <c r="C8" s="16" t="s">
+        <v>30</v>
+      </c>
+      <c r="D8" s="17" t="s">
         <v>76</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A9" s="19" t="s">
+      <c r="A9" s="16" t="s">
         <v>78</v>
       </c>
-      <c r="B9" s="19" t="s">
-        <v>27</v>
-      </c>
-      <c r="C9" s="19" t="s">
-        <v>30</v>
-      </c>
-      <c r="D9" s="20" t="s">
+      <c r="B9" s="16" t="s">
+        <v>27</v>
+      </c>
+      <c r="C9" s="16" t="s">
+        <v>30</v>
+      </c>
+      <c r="D9" s="17" t="s">
         <v>75</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A10" s="19" t="s">
+      <c r="A10" s="16" t="s">
         <v>79</v>
       </c>
-      <c r="B10" s="19" t="s">
-        <v>27</v>
-      </c>
-      <c r="C10" s="19" t="s">
-        <v>30</v>
-      </c>
-      <c r="D10" s="19" t="s">
+      <c r="B10" s="16" t="s">
+        <v>27</v>
+      </c>
+      <c r="C10" s="16" t="s">
+        <v>30</v>
+      </c>
+      <c r="D10" s="16" t="s">
         <v>80</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A11" s="19" t="s">
+      <c r="A11" s="16" t="s">
         <v>82</v>
       </c>
-      <c r="B11" s="19" t="s">
-        <v>27</v>
-      </c>
-      <c r="C11" s="19" t="s">
-        <v>30</v>
-      </c>
-      <c r="D11" s="19" t="s">
+      <c r="B11" s="16" t="s">
+        <v>27</v>
+      </c>
+      <c r="C11" s="16" t="s">
+        <v>30</v>
+      </c>
+      <c r="D11" s="16" t="s">
         <v>83</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A12" s="18" t="s">
+      <c r="A12" s="15" t="s">
         <v>85</v>
       </c>
-      <c r="B12" s="18" t="s">
-        <v>27</v>
-      </c>
-      <c r="C12" s="18" t="s">
-        <v>30</v>
-      </c>
-      <c r="D12" s="22" t="s">
+      <c r="B12" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="C12" s="15" t="s">
+        <v>30</v>
+      </c>
+      <c r="D12" s="19" t="s">
         <v>90</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A13" s="18" t="s">
+      <c r="A13" s="15" t="s">
         <v>86</v>
       </c>
-      <c r="B13" s="18" t="s">
-        <v>27</v>
-      </c>
-      <c r="C13" s="18" t="s">
-        <v>30</v>
-      </c>
-      <c r="D13" s="22" t="s">
+      <c r="B13" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="C13" s="15" t="s">
+        <v>30</v>
+      </c>
+      <c r="D13" s="19" t="s">
         <v>91</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A14" s="18" t="s">
+      <c r="A14" s="15" t="s">
         <v>87</v>
       </c>
-      <c r="B14" s="18" t="s">
-        <v>27</v>
-      </c>
-      <c r="C14" s="18" t="s">
-        <v>30</v>
-      </c>
-      <c r="D14" s="18" t="s">
+      <c r="B14" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="C14" s="15" t="s">
+        <v>30</v>
+      </c>
+      <c r="D14" s="15" t="s">
         <v>92</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A15" s="18" t="s">
+      <c r="A15" s="15" t="s">
         <v>88</v>
       </c>
-      <c r="B15" s="18" t="s">
-        <v>27</v>
-      </c>
-      <c r="C15" s="18" t="s">
-        <v>30</v>
-      </c>
-      <c r="D15" s="18" t="s">
+      <c r="B15" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="C15" s="15" t="s">
+        <v>30</v>
+      </c>
+      <c r="D15" s="15" t="s">
         <v>89</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A16" s="19" t="s">
+      <c r="A16" s="16" t="s">
         <v>93</v>
       </c>
-      <c r="B16" s="19" t="s">
-        <v>27</v>
-      </c>
-      <c r="C16" s="19" t="s">
-        <v>30</v>
-      </c>
-      <c r="D16" s="20" t="s">
+      <c r="B16" s="16" t="s">
+        <v>27</v>
+      </c>
+      <c r="C16" s="16" t="s">
+        <v>30</v>
+      </c>
+      <c r="D16" s="17" t="s">
         <v>97</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A17" s="19" t="s">
+      <c r="A17" s="16" t="s">
         <v>94</v>
       </c>
-      <c r="B17" s="19" t="s">
-        <v>27</v>
-      </c>
-      <c r="C17" s="19" t="s">
-        <v>30</v>
-      </c>
-      <c r="D17" s="20" t="s">
+      <c r="B17" s="16" t="s">
+        <v>27</v>
+      </c>
+      <c r="C17" s="16" t="s">
+        <v>30</v>
+      </c>
+      <c r="D17" s="17" t="s">
         <v>98</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A18" s="19" t="s">
+      <c r="A18" s="16" t="s">
         <v>95</v>
       </c>
-      <c r="B18" s="19" t="s">
-        <v>27</v>
-      </c>
-      <c r="C18" s="19" t="s">
-        <v>30</v>
-      </c>
-      <c r="D18" s="19" t="s">
+      <c r="B18" s="16" t="s">
+        <v>27</v>
+      </c>
+      <c r="C18" s="16" t="s">
+        <v>30</v>
+      </c>
+      <c r="D18" s="16" t="s">
         <v>81</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A19" s="19" t="s">
+      <c r="A19" s="16" t="s">
         <v>96</v>
       </c>
-      <c r="B19" s="19" t="s">
-        <v>27</v>
-      </c>
-      <c r="C19" s="19" t="s">
-        <v>30</v>
-      </c>
-      <c r="D19" s="19" t="s">
+      <c r="B19" s="16" t="s">
+        <v>27</v>
+      </c>
+      <c r="C19" s="16" t="s">
+        <v>30</v>
+      </c>
+      <c r="D19" s="16" t="s">
         <v>84</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A20" s="18" t="s">
+      <c r="A20" s="15" t="s">
         <v>100</v>
       </c>
-      <c r="B20" s="18" t="s">
-        <v>27</v>
-      </c>
-      <c r="C20" s="18" t="s">
-        <v>30</v>
-      </c>
-      <c r="D20" s="22" t="s">
+      <c r="B20" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="C20" s="15" t="s">
+        <v>30</v>
+      </c>
+      <c r="D20" s="19" t="s">
         <v>99</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A21" s="19" t="s">
+      <c r="A21" s="16" t="s">
         <v>101</v>
       </c>
-      <c r="B21" s="19" t="s">
-        <v>27</v>
-      </c>
-      <c r="C21" s="19" t="s">
-        <v>30</v>
-      </c>
-      <c r="D21" s="20" t="s">
+      <c r="B21" s="16" t="s">
+        <v>27</v>
+      </c>
+      <c r="C21" s="16" t="s">
+        <v>30</v>
+      </c>
+      <c r="D21" s="17" t="s">
         <v>102</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A22" s="19" t="s">
+      <c r="A22" s="16" t="s">
         <v>103</v>
       </c>
-      <c r="B22" s="19" t="s">
-        <v>27</v>
-      </c>
-      <c r="C22" s="19" t="s">
-        <v>30</v>
-      </c>
-      <c r="D22" s="19" t="s">
+      <c r="B22" s="16" t="s">
+        <v>27</v>
+      </c>
+      <c r="C22" s="16" t="s">
+        <v>30</v>
+      </c>
+      <c r="D22" s="16" t="s">
         <v>104</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A23" s="18" t="s">
+      <c r="A23" s="15" t="s">
         <v>42</v>
       </c>
-      <c r="B23" s="18" t="s">
-        <v>27</v>
-      </c>
-      <c r="C23" s="18" t="s">
-        <v>30</v>
-      </c>
-      <c r="D23" s="18" t="s">
+      <c r="B23" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="C23" s="15" t="s">
+        <v>30</v>
+      </c>
+      <c r="D23" s="15" t="s">
         <v>105</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A25" s="24" t="s">
+      <c r="A25" s="21" t="s">
         <v>34</v>
       </c>
-      <c r="B25" s="23" t="s">
+      <c r="B25" s="20" t="s">
         <v>116</v>
       </c>
     </row>
@@ -1791,7 +1817,7 @@
       <c r="C28" t="s">
         <v>30</v>
       </c>
-      <c r="D28" s="13" t="s">
+      <c r="D28" s="10" t="s">
         <v>108</v>
       </c>
       <c r="E28" t="s">
@@ -1808,7 +1834,7 @@
       <c r="C29" t="s">
         <v>32</v>
       </c>
-      <c r="D29" s="13" t="s">
+      <c r="D29" s="10" t="s">
         <v>109</v>
       </c>
       <c r="E29" t="s">
@@ -1816,10 +1842,10 @@
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A31" s="24" t="s">
+      <c r="A31" s="21" t="s">
         <v>41</v>
       </c>
-      <c r="B31" s="23" t="s">
+      <c r="B31" s="20" t="s">
         <v>115</v>
       </c>
     </row>
@@ -1892,41 +1918,41 @@
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A36" s="7" t="s">
+      <c r="A36" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="B36" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="C36" s="8" t="s">
-        <v>30</v>
-      </c>
-      <c r="D36" s="13" t="s">
+      <c r="B36" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="C36" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="D36" s="10" t="s">
         <v>113</v>
       </c>
-      <c r="E36" s="9" t="s">
+      <c r="E36" s="6" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A37" s="7" t="s">
+      <c r="A37" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="B37" s="8" t="s">
+      <c r="B37" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="C37" s="8" t="s">
+      <c r="C37" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="D37" s="13" t="s">
+      <c r="D37" s="10" t="s">
         <v>114</v>
       </c>
-      <c r="E37" s="9" t="s">
+      <c r="E37" s="6" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A39" s="21" t="s">
+      <c r="A39" s="18" t="s">
         <v>45</v>
       </c>
     </row>
@@ -1957,7 +1983,7 @@
       <c r="C41" t="s">
         <v>35</v>
       </c>
-      <c r="D41" s="14"/>
+      <c r="D41" s="11"/>
       <c r="E41" t="s">
         <v>38</v>
       </c>
@@ -1972,7 +1998,7 @@
       <c r="C42" t="s">
         <v>35</v>
       </c>
-      <c r="D42" s="14"/>
+      <c r="D42" s="11"/>
       <c r="E42" t="s">
         <v>38</v>
       </c>
@@ -1987,7 +2013,7 @@
       <c r="C43" t="s">
         <v>35</v>
       </c>
-      <c r="D43" s="14"/>
+      <c r="D43" s="11"/>
       <c r="E43" t="s">
         <v>38</v>
       </c>
@@ -2002,43 +2028,43 @@
       <c r="C44" t="s">
         <v>35</v>
       </c>
-      <c r="D44" s="14"/>
+      <c r="D44" s="11"/>
       <c r="E44" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A45" s="7" t="s">
+      <c r="A45" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="B45" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="C45" s="8" t="s">
+      <c r="B45" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="C45" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="D45" s="15"/>
-      <c r="E45" s="9" t="s">
+      <c r="D45" s="12"/>
+      <c r="E45" s="6" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A46" s="7" t="s">
+      <c r="A46" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="B46" s="8" t="s">
+      <c r="B46" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="C46" s="8" t="s">
+      <c r="C46" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="D46" s="15"/>
-      <c r="E46" s="9" t="s">
+      <c r="D46" s="12"/>
+      <c r="E46" s="6" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A48" s="21" t="s">
+      <c r="A48" s="18" t="s">
         <v>50</v>
       </c>
     </row>
@@ -2069,7 +2095,7 @@
       <c r="C50" t="s">
         <v>35</v>
       </c>
-      <c r="D50" s="17" t="s">
+      <c r="D50" s="14" t="s">
         <v>63</v>
       </c>
       <c r="E50" t="s">
@@ -2077,32 +2103,32 @@
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A51" s="7" t="s">
+      <c r="A51" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="B51" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="C51" s="8" t="s">
+      <c r="B51" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="C51" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="D51" s="16"/>
-      <c r="E51" s="9" t="s">
+      <c r="D51" s="13"/>
+      <c r="E51" s="6" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A52" s="7" t="s">
+      <c r="A52" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="B52" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="C52" s="8" t="s">
+      <c r="B52" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="C52" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="D52" s="17"/>
-      <c r="E52" s="9" t="s">
+      <c r="D52" s="14"/>
+      <c r="E52" s="6" t="s">
         <v>38</v>
       </c>
     </row>
@@ -2116,7 +2142,7 @@
       <c r="C53" t="s">
         <v>35</v>
       </c>
-      <c r="D53" s="17"/>
+      <c r="D53" s="14"/>
       <c r="E53" t="s">
         <v>38</v>
       </c>
@@ -2131,7 +2157,7 @@
       <c r="C54" t="s">
         <v>35</v>
       </c>
-      <c r="D54" s="17" t="s">
+      <c r="D54" s="14" t="s">
         <v>64</v>
       </c>
       <c r="E54" t="s">
@@ -2139,41 +2165,41 @@
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A55" s="7" t="s">
+      <c r="A55" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="B55" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="C55" s="8" t="s">
+      <c r="B55" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="C55" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="D55" s="17" t="s">
+      <c r="D55" s="14" t="s">
         <v>65</v>
       </c>
-      <c r="E55" s="9" t="s">
+      <c r="E55" s="6" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A56" s="7" t="s">
+      <c r="A56" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="B56" s="8" t="s">
+      <c r="B56" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="C56" s="8" t="s">
+      <c r="C56" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="D56" s="17" t="s">
+      <c r="D56" s="14" t="s">
         <v>60</v>
       </c>
-      <c r="E56" s="9" t="s">
+      <c r="E56" s="6" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A58" s="24" t="s">
+      <c r="A58" s="21" t="s">
         <v>54</v>
       </c>
       <c r="B58" t="s">
@@ -2249,53 +2275,53 @@
       </c>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A63" s="7" t="s">
+      <c r="A63" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="B63" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="C63" s="8" t="s">
-        <v>30</v>
-      </c>
-      <c r="D63" s="13" t="s">
+      <c r="B63" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="C63" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="D63" s="10" t="s">
         <v>129</v>
       </c>
-      <c r="E63" s="9" t="s">
+      <c r="E63" s="6" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A64" s="10" t="s">
+      <c r="A64" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="B64" s="11" t="s">
+      <c r="B64" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="C64" s="11" t="s">
+      <c r="C64" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="D64" s="13" t="s">
+      <c r="D64" s="10" t="s">
         <v>130</v>
       </c>
-      <c r="E64" s="12" t="s">
+      <c r="E64" s="9" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A65" s="25" t="s">
+      <c r="A65" t="s">
         <v>123</v>
       </c>
-      <c r="B65" s="25" t="s">
-        <v>27</v>
-      </c>
-      <c r="C65" s="25" t="s">
-        <v>30</v>
-      </c>
-      <c r="D65" s="25" t="s">
+      <c r="B65" t="s">
+        <v>27</v>
+      </c>
+      <c r="C65" t="s">
+        <v>30</v>
+      </c>
+      <c r="D65" t="s">
         <v>124</v>
       </c>
-      <c r="E65" s="25" t="s">
+      <c r="E65" t="s">
         <v>38</v>
       </c>
     </row>
@@ -2334,10 +2360,10 @@
       </c>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A69" s="24" t="s">
+      <c r="A69" s="21" t="s">
         <v>53</v>
       </c>
-      <c r="B69" s="23" t="s">
+      <c r="B69" s="20" t="s">
         <v>117</v>
       </c>
     </row>
@@ -2368,7 +2394,7 @@
       <c r="C71" t="s">
         <v>30</v>
       </c>
-      <c r="D71" s="13" t="s">
+      <c r="D71" s="10" t="s">
         <v>67</v>
       </c>
       <c r="E71" t="s">
@@ -2385,7 +2411,7 @@
       <c r="C72" t="s">
         <v>30</v>
       </c>
-      <c r="D72" s="13" t="s">
+      <c r="D72" s="10" t="s">
         <v>118</v>
       </c>
       <c r="E72" t="s">
@@ -2393,70 +2419,70 @@
       </c>
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A73" s="7" t="s">
+      <c r="A73" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="B73" s="8" t="s">
+      <c r="B73" s="5" t="s">
         <v>27</v>
       </c>
       <c r="C73" t="s">
         <v>30</v>
       </c>
-      <c r="D73" s="13" t="s">
+      <c r="D73" s="10" t="s">
         <v>73</v>
       </c>
-      <c r="E73" s="9" t="s">
+      <c r="E73" s="6" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A74" s="7" t="s">
+      <c r="A74" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="B74" s="8" t="s">
+      <c r="B74" s="5" t="s">
         <v>27</v>
       </c>
       <c r="C74" t="s">
         <v>30</v>
       </c>
-      <c r="D74" s="13" t="s">
+      <c r="D74" s="10" t="s">
         <v>121</v>
       </c>
-      <c r="E74" s="9" t="s">
+      <c r="E74" s="6" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A75" s="7" t="s">
+      <c r="A75" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="B75" s="8" t="s">
+      <c r="B75" s="5" t="s">
         <v>27</v>
       </c>
       <c r="C75" t="s">
         <v>30</v>
       </c>
-      <c r="D75" s="13" t="s">
+      <c r="D75" s="10" t="s">
         <v>119</v>
       </c>
-      <c r="E75" s="9" t="s">
+      <c r="E75" s="6" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A76" s="7" t="s">
+      <c r="A76" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="B76" s="8" t="s">
+      <c r="B76" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="C76" s="8" t="s">
+      <c r="C76" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="D76" s="13" t="s">
+      <c r="D76" s="10" t="s">
         <v>120</v>
       </c>
-      <c r="E76" s="9" t="s">
+      <c r="E76" s="6" t="s">
         <v>39</v>
       </c>
     </row>
@@ -2477,99 +2503,123 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7302641A-0A23-4DC3-9DD6-B859F68A38DB}">
-  <dimension ref="A3:G5"/>
+  <dimension ref="A3:G6"/>
   <sheetViews>
-    <sheetView topLeftCell="B5" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="13.6328125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11.54296875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="27.453125" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="59.08984375" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="7" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="26.90625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="37.6328125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="58.7265625" customWidth="1"/>
     <col min="7" max="7" width="57.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="5" t="s">
+    <row r="3" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="5" t="s">
+      <c r="B3" s="22" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="5" t="s">
+      <c r="C3" s="22" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="5" t="s">
+      <c r="D3" s="22" t="s">
         <v>6</v>
       </c>
-      <c r="E3" s="5" t="s">
+      <c r="E3" s="22" t="s">
         <v>7</v>
       </c>
-      <c r="F3" s="5" t="s">
+      <c r="F3" s="22" t="s">
         <v>12</v>
       </c>
-      <c r="G3" s="5" t="s">
+      <c r="G3" s="22" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:7" s="2" customFormat="1" ht="116" x14ac:dyDescent="0.35">
-      <c r="A4" s="2" t="s">
+    <row r="4" spans="1:7" s="1" customFormat="1" ht="116" x14ac:dyDescent="0.35">
+      <c r="A4" s="23" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="B4" s="23" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="C4" s="24" t="s">
         <v>15</v>
       </c>
-      <c r="D4" s="2" t="s">
+      <c r="D4" s="23" t="s">
         <v>13</v>
       </c>
-      <c r="E4" s="2" t="s">
+      <c r="E4" s="23" t="s">
         <v>8</v>
       </c>
-      <c r="F4" s="3" t="s">
+      <c r="F4" s="25" t="s">
         <v>9</v>
       </c>
-      <c r="G4" s="4" t="s">
+      <c r="G4" s="26" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:7" s="2" customFormat="1" ht="130.5" x14ac:dyDescent="0.35">
-      <c r="A5" s="2" t="s">
+    <row r="5" spans="1:7" s="1" customFormat="1" ht="130.5" x14ac:dyDescent="0.35">
+      <c r="A5" s="23" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="B5" s="23" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="1" t="s">
+      <c r="C5" s="24" t="s">
         <v>15</v>
       </c>
-      <c r="D5" s="2" t="s">
+      <c r="D5" s="23" t="s">
         <v>13</v>
       </c>
-      <c r="E5" s="2" t="s">
+      <c r="E5" s="23" t="s">
         <v>8</v>
       </c>
-      <c r="F5" s="2" t="s">
+      <c r="F5" s="23" t="s">
         <v>13</v>
       </c>
-      <c r="G5" s="3" t="s">
+      <c r="G5" s="25" t="s">
         <v>14</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="87" x14ac:dyDescent="0.35">
+      <c r="A6" s="23" t="s">
+        <v>133</v>
+      </c>
+      <c r="B6" s="23" t="s">
+        <v>5</v>
+      </c>
+      <c r="C6" s="24" t="s">
+        <v>132</v>
+      </c>
+      <c r="D6" s="23" t="s">
+        <v>13</v>
+      </c>
+      <c r="E6" s="23" t="s">
+        <v>8</v>
+      </c>
+      <c r="F6" s="25" t="s">
+        <v>134</v>
+      </c>
+      <c r="G6" s="25" t="s">
+        <v>135</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="C4" r:id="rId1" xr:uid="{ECC5B591-8991-45F0-AFDE-52BAB35D6900}"/>
     <hyperlink ref="C5" r:id="rId2" xr:uid="{274C0DE0-C21F-4341-9397-4CA8B40F8613}"/>
+    <hyperlink ref="C6" r:id="rId3" xr:uid="{7B404CB7-A5DC-42F3-A632-B8E9503779E1}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId4"/>
 </worksheet>
 </file>
 
@@ -2578,7 +2628,7 @@
   <dimension ref="A2:C5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="A2:C5"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>

<commit_message>
Endpoint for table update
</commit_message>
<xml_diff>
--- a/Endpoints.xlsx
+++ b/Endpoints.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Environment\DEV\Documentation\stock-project-documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86D97E17-EDEF-4A60-88EA-0247C919C913}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C0D7148-2E1D-4B1F-8122-61362A50B601}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{30700010-F763-4196-BFD8-63DDF9783492}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="1" xr2:uid="{30700010-F763-4196-BFD8-63DDF9783492}"/>
   </bookViews>
   <sheets>
     <sheet name="Summary Page" sheetId="3" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="333" uniqueCount="136">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="340" uniqueCount="140">
   <si>
     <t>Class</t>
   </si>
@@ -101,9 +101,6 @@
     },                                                                                                                               ]</t>
   </si>
   <si>
-    <t>http://localhost:8080/v1/stocks</t>
-  </si>
-  <si>
     <t>MarketController</t>
   </si>
   <si>
@@ -450,9 +447,6 @@
   </si>
   <si>
     <t>"/profit-loss-dashboard" API</t>
-  </si>
-  <si>
-    <t>http://localhost:8080/stock-app/v1/company-dropdowns/with-excel</t>
   </si>
   <si>
     <t>CompanyNameDropdownController</t>
@@ -471,6 +465,33 @@
         "companySymbol": "20MICRONS",
         "companyName": "20 Microns Limited"
     },                                                                                                                      ]</t>
+  </si>
+  <si>
+    <t>http://localhost:8085/stock-app/v1/stocks</t>
+  </si>
+  <si>
+    <t>http://localhost:8085/stock-app/v1/company-dropdowns/with-excel</t>
+  </si>
+  <si>
+    <t>http://localhost:8085/stock-app/v1/misc-records</t>
+  </si>
+  <si>
+    <t>PUT</t>
+  </si>
+  <si>
+    <t>MiscellaneousRecordController</t>
+  </si>
+  <si>
+    <t>{
+    "miscId": "MASTER-KEY",
+    "cashAvailableForInvesting": 0.0,
+    "stockTableUpdatedOn": "2020-01-23",
+    "mutualFundTableUpdatedOn": "2020-01-18",
+    "fundTableUpdatedOn": "2020-01-18",
+    "dividendTableUpdatedOn": "2020-01-18",
+    "profitLossTableUpdatedOn": "2020-01-18",
+    "goldTableUpdatedOn": "2020-01-18"
+}</t>
   </si>
 </sst>
 </file>
@@ -674,7 +695,7 @@
     <xf numFmtId="0" fontId="4" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -717,6 +738,12 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="8">
@@ -1439,7 +1466,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3EF971A8-AD54-4406-A028-7A2295393BC1}">
   <dimension ref="A1:E76"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D58" sqref="D58"/>
     </sheetView>
   </sheetViews>
@@ -1454,1036 +1481,1036 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" s="16" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B3" s="16" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C3" s="16" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D3" s="16" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4" s="15" t="s">
+        <v>67</v>
+      </c>
+      <c r="B4" s="15" t="s">
+        <v>26</v>
+      </c>
+      <c r="C4" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="D4" s="15" t="s">
         <v>68</v>
-      </c>
-      <c r="B4" s="15" t="s">
-        <v>27</v>
-      </c>
-      <c r="C4" s="15" t="s">
-        <v>30</v>
-      </c>
-      <c r="D4" s="15" t="s">
-        <v>69</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A5" s="15" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B5" s="15" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C5" s="15" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D5" s="15" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A6" s="15" t="s">
+        <v>70</v>
+      </c>
+      <c r="B6" s="15" t="s">
+        <v>26</v>
+      </c>
+      <c r="C6" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="D6" s="15" t="s">
         <v>71</v>
-      </c>
-      <c r="B6" s="15" t="s">
-        <v>27</v>
-      </c>
-      <c r="C6" s="15" t="s">
-        <v>30</v>
-      </c>
-      <c r="D6" s="15" t="s">
-        <v>72</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A7" s="15" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B7" s="15" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C7" s="15" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D7" s="15" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A8" s="16" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B8" s="16" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C8" s="16" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D8" s="17" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A9" s="16" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B9" s="16" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C9" s="16" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D9" s="17" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A10" s="16" t="s">
+        <v>78</v>
+      </c>
+      <c r="B10" s="16" t="s">
+        <v>26</v>
+      </c>
+      <c r="C10" s="16" t="s">
+        <v>29</v>
+      </c>
+      <c r="D10" s="16" t="s">
         <v>79</v>
-      </c>
-      <c r="B10" s="16" t="s">
-        <v>27</v>
-      </c>
-      <c r="C10" s="16" t="s">
-        <v>30</v>
-      </c>
-      <c r="D10" s="16" t="s">
-        <v>80</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A11" s="16" t="s">
+        <v>81</v>
+      </c>
+      <c r="B11" s="16" t="s">
+        <v>26</v>
+      </c>
+      <c r="C11" s="16" t="s">
+        <v>29</v>
+      </c>
+      <c r="D11" s="16" t="s">
         <v>82</v>
-      </c>
-      <c r="B11" s="16" t="s">
-        <v>27</v>
-      </c>
-      <c r="C11" s="16" t="s">
-        <v>30</v>
-      </c>
-      <c r="D11" s="16" t="s">
-        <v>83</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A12" s="15" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B12" s="15" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C12" s="15" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D12" s="19" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A13" s="15" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B13" s="15" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C13" s="15" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D13" s="19" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A14" s="15" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B14" s="15" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C14" s="15" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D14" s="15" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A15" s="15" t="s">
+        <v>87</v>
+      </c>
+      <c r="B15" s="15" t="s">
+        <v>26</v>
+      </c>
+      <c r="C15" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="D15" s="15" t="s">
         <v>88</v>
-      </c>
-      <c r="B15" s="15" t="s">
-        <v>27</v>
-      </c>
-      <c r="C15" s="15" t="s">
-        <v>30</v>
-      </c>
-      <c r="D15" s="15" t="s">
-        <v>89</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A16" s="16" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B16" s="16" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C16" s="16" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D16" s="17" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A17" s="16" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B17" s="16" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C17" s="16" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D17" s="17" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A18" s="16" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B18" s="16" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C18" s="16" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D18" s="16" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A19" s="16" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B19" s="16" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C19" s="16" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D19" s="16" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A20" s="15" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B20" s="15" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C20" s="15" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D20" s="19" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A21" s="16" t="s">
+        <v>100</v>
+      </c>
+      <c r="B21" s="16" t="s">
+        <v>26</v>
+      </c>
+      <c r="C21" s="16" t="s">
+        <v>29</v>
+      </c>
+      <c r="D21" s="17" t="s">
         <v>101</v>
-      </c>
-      <c r="B21" s="16" t="s">
-        <v>27</v>
-      </c>
-      <c r="C21" s="16" t="s">
-        <v>30</v>
-      </c>
-      <c r="D21" s="17" t="s">
-        <v>102</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A22" s="16" t="s">
+        <v>102</v>
+      </c>
+      <c r="B22" s="16" t="s">
+        <v>26</v>
+      </c>
+      <c r="C22" s="16" t="s">
+        <v>29</v>
+      </c>
+      <c r="D22" s="16" t="s">
         <v>103</v>
-      </c>
-      <c r="B22" s="16" t="s">
-        <v>27</v>
-      </c>
-      <c r="C22" s="16" t="s">
-        <v>30</v>
-      </c>
-      <c r="D22" s="16" t="s">
-        <v>104</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A23" s="15" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B23" s="15" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C23" s="15" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D23" s="15" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A25" s="21" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B25" s="20" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B26" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C26" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D26" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E26" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
+        <v>105</v>
+      </c>
+      <c r="B27" t="s">
+        <v>26</v>
+      </c>
+      <c r="C27" t="s">
+        <v>29</v>
+      </c>
+      <c r="D27" t="s">
         <v>106</v>
       </c>
-      <c r="B27" t="s">
-        <v>27</v>
-      </c>
-      <c r="C27" t="s">
-        <v>30</v>
-      </c>
-      <c r="D27" t="s">
-        <v>107</v>
-      </c>
       <c r="E27" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B28" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C28" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D28" s="10" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="E28" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B29" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C29" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D29" s="10" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="E29" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A31" s="21" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B31" s="20" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B32" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C32" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D32" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E32" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B33" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C33" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D33" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="E33" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B34" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C34" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D34" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="E34" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B35" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C35" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D35" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E35" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A36" s="4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B36" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C36" s="5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D36" s="10" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="E36" s="6" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A37" s="4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B37" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C37" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D37" s="10" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="E37" s="6" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A39" s="18" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B40" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C40" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D40" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E40" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B41" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C41" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D41" s="11"/>
       <c r="E41" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B42" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C42" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D42" s="11"/>
       <c r="E42" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B43" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C43" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D43" s="11"/>
       <c r="E43" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B44" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C44" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D44" s="11"/>
       <c r="E44" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A45" s="4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B45" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C45" s="5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D45" s="12"/>
       <c r="E45" s="6" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A46" s="4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B46" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C46" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D46" s="12"/>
       <c r="E46" s="6" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A48" s="18" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B49" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C49" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D49" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E49" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B50" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C50" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D50" s="14" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E50" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A51" s="4" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B51" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C51" s="5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D51" s="13"/>
       <c r="E51" s="6" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A52" s="4" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B52" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C52" s="5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D52" s="14"/>
       <c r="E52" s="6" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A53" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B53" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C53" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D53" s="14"/>
       <c r="E53" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A54" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B54" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C54" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D54" s="14" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E54" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A55" s="4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B55" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C55" s="5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D55" s="14" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E55" s="6" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A56" s="4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B56" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C56" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D56" s="14" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E56" s="6" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A58" s="21" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B58" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A59" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B59" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C59" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D59" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E59" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A60" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B60" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C60" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D60" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="E60" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A61" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B61" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C61" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D61" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="E61" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A62" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B62" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C62" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D62" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="E62" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A63" s="4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B63" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C63" s="5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D63" s="10" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="E63" s="6" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A64" s="7" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B64" s="8" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C64" s="8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D64" s="10" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="E64" s="9" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A65" t="s">
+        <v>122</v>
+      </c>
+      <c r="B65" t="s">
+        <v>26</v>
+      </c>
+      <c r="C65" t="s">
+        <v>29</v>
+      </c>
+      <c r="D65" t="s">
         <v>123</v>
       </c>
-      <c r="B65" t="s">
-        <v>27</v>
-      </c>
-      <c r="C65" t="s">
-        <v>30</v>
-      </c>
-      <c r="D65" t="s">
-        <v>124</v>
-      </c>
       <c r="E65" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A66" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B66" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C66" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D66" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="E66" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A67" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B67" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C67" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D67" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="E67" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A69" s="21" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B69" s="20" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A70" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B70" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C70" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D70" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E70" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A71" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B71" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C71" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D71" s="10" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E71" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A72" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B72" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C72" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D72" s="10" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="E72" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A73" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B73" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C73" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D73" s="10" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E73" s="6" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A74" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B74" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C74" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D74" s="10" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="E74" s="6" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A75" s="4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B75" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C75" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D75" s="10" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="E75" s="6" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A76" s="4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B76" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C76" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D76" s="10" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="E76" s="6" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
   </sheetData>
@@ -2503,15 +2530,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7302641A-0A23-4DC3-9DD6-B859F68A38DB}">
-  <dimension ref="A3:G6"/>
+  <dimension ref="A3:G7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="13.6328125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="21.90625" customWidth="1"/>
     <col min="2" max="2" width="11.54296875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="59.08984375" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="7" bestFit="1" customWidth="1"/>
@@ -2551,7 +2578,7 @@
         <v>5</v>
       </c>
       <c r="C4" s="24" t="s">
-        <v>15</v>
+        <v>134</v>
       </c>
       <c r="D4" s="23" t="s">
         <v>13</v>
@@ -2574,7 +2601,7 @@
         <v>4</v>
       </c>
       <c r="C5" s="24" t="s">
-        <v>15</v>
+        <v>134</v>
       </c>
       <c r="D5" s="23" t="s">
         <v>13</v>
@@ -2591,13 +2618,13 @@
     </row>
     <row r="6" spans="1:7" ht="87" x14ac:dyDescent="0.35">
       <c r="A6" s="23" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="B6" s="23" t="s">
         <v>5</v>
       </c>
       <c r="C6" s="24" t="s">
-        <v>132</v>
+        <v>135</v>
       </c>
       <c r="D6" s="23" t="s">
         <v>13</v>
@@ -2606,10 +2633,33 @@
         <v>8</v>
       </c>
       <c r="F6" s="25" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="G6" s="25" t="s">
-        <v>135</v>
+        <v>133</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="145" x14ac:dyDescent="0.35">
+      <c r="A7" s="23" t="s">
+        <v>138</v>
+      </c>
+      <c r="B7" s="23" t="s">
+        <v>137</v>
+      </c>
+      <c r="C7" s="28" t="s">
+        <v>136</v>
+      </c>
+      <c r="D7" s="23" t="s">
+        <v>13</v>
+      </c>
+      <c r="E7" s="23" t="s">
+        <v>8</v>
+      </c>
+      <c r="F7" s="27" t="s">
+        <v>139</v>
+      </c>
+      <c r="G7" s="27" t="s">
+        <v>139</v>
       </c>
     </row>
   </sheetData>
@@ -2617,9 +2667,10 @@
     <hyperlink ref="C4" r:id="rId1" xr:uid="{ECC5B591-8991-45F0-AFDE-52BAB35D6900}"/>
     <hyperlink ref="C5" r:id="rId2" xr:uid="{274C0DE0-C21F-4341-9397-4CA8B40F8613}"/>
     <hyperlink ref="C6" r:id="rId3" xr:uid="{7B404CB7-A5DC-42F3-A632-B8E9503779E1}"/>
+    <hyperlink ref="C7" r:id="rId4" xr:uid="{AA0702AF-1C91-4984-89BB-D839831D209A}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId4"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId5"/>
 </worksheet>
 </file>
 
@@ -2640,7 +2691,7 @@
   <sheetData>
     <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.35">
@@ -2648,10 +2699,10 @@
         <v>4</v>
       </c>
       <c r="B3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.35">
@@ -2659,10 +2710,10 @@
         <v>4</v>
       </c>
       <c r="B4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.35">
@@ -2670,10 +2721,10 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>